<commit_message>
Edit BOD san Meals
</commit_message>
<xml_diff>
--- a/Mapping Matrix update.xlsx
+++ b/Mapping Matrix update.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sy\Downloads\Compressed\cloneBr\clone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07EF9874-F860-49DF-ACA3-B1BFBE0CFC26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24442020-72AA-49C8-AB68-1108F5E7F1C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PICemail &amp; WTprefix" sheetId="1" r:id="rId1"/>
@@ -1687,18 +1687,12 @@
     <t>ISAT 25 AGUSTUS 2020;AGUSTUS 2020 OK;0;Master data;0;Sheet1;New Hire;Meals;Musibah;Nikah;Khitan</t>
   </si>
   <si>
-    <t>C10:AC;B9:D;0;B2:J;0;C2:F;D5:O;A4:F;D2:L;B2:K;B2:H</t>
-  </si>
-  <si>
     <t>8;8;0;1;0;1;4;3;1;1;1</t>
   </si>
   <si>
     <t>4004,4005,4006,4007;4026;0;4001;0;2135;1000,1005,1010;2285;2060;2160;2190</t>
   </si>
   <si>
-    <t>0,23,24,25,26;0,2,91,92,93;91,92,93,94,95;0,6,7,8,93;91,92,93,94,95;0,3,91,92,93;0,9,10,11,99;0,5,93,94,95;0,8,91,92,93;0,1,91,92,93;0,1,91,92,93</t>
-  </si>
-  <si>
     <t>BOD</t>
   </si>
   <si>
@@ -1706,6 +1700,12 @@
   </si>
   <si>
     <t>D:\PrePayroll\2020\11\External\BOD</t>
+  </si>
+  <si>
+    <t>C10:AC;B9:D;0;B2:J;0;C2:F;B5:O;A4:F;D2:L;B2:K;B2:H</t>
+  </si>
+  <si>
+    <t>0,23,24,25,26;0,2,91,92,93;91,92,93,94,95;0,6,7,8,93;91,92,93,94,95;0,3,91,92,93;0,11,12,13,99;0,5,93,94,95;0,8,91,92,93;0,1,91,92,93;0,1,91,92,93</t>
   </si>
 </sst>
 </file>
@@ -1729,57 +1729,67 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -1855,7 +1865,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1901,6 +1911,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2161,7 +2172,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
@@ -2635,7 +2646,7 @@
         <v>540</v>
       </c>
       <c r="H29" s="26" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2643,16 +2654,16 @@
         <v>12</v>
       </c>
       <c r="B30" s="25" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C30" s="30" t="s">
         <v>513</v>
       </c>
       <c r="D30" t="s">
+        <v>553</v>
+      </c>
+      <c r="H30" s="26" t="s">
         <v>555</v>
-      </c>
-      <c r="H30" s="26" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3637,8 +3648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A4:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3692,7 +3703,7 @@
         <v>166</v>
       </c>
       <c r="B9" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -3707,16 +3718,16 @@
       <c r="A11" t="s">
         <v>523</v>
       </c>
-      <c r="B11" t="s">
-        <v>551</v>
+      <c r="B11" s="31" t="s">
+        <v>556</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>524</v>
       </c>
-      <c r="B12" t="s">
-        <v>554</v>
+      <c r="B12" s="31" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -3724,7 +3735,7 @@
         <v>525</v>
       </c>
       <c r="B13" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update Program laptop Indosat
</commit_message>
<xml_diff>
--- a/Mapping Matrix update.xlsx
+++ b/Mapping Matrix update.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sy\Downloads\Compressed\cloneBr\clone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24442020-72AA-49C8-AB68-1108F5E7F1C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D67D1B07-DC88-460E-BAD9-06A944DCD160}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1612,9 +1612,6 @@
     <t>Penambah Cell</t>
   </si>
   <si>
-    <t>1000000;300000</t>
-  </si>
-  <si>
     <t>List Amount</t>
   </si>
   <si>
@@ -1684,15 +1681,6 @@
     <t>syahid.alirfan@outlook.co.id</t>
   </si>
   <si>
-    <t>ISAT 25 AGUSTUS 2020;AGUSTUS 2020 OK;0;Master data;0;Sheet1;New Hire;Meals;Musibah;Nikah;Khitan</t>
-  </si>
-  <si>
-    <t>8;8;0;1;0;1;4;3;1;1;1</t>
-  </si>
-  <si>
-    <t>4004,4005,4006,4007;4026;0;4001;0;2135;1000,1005,1010;2285;2060;2160;2190</t>
-  </si>
-  <si>
     <t>BOD</t>
   </si>
   <si>
@@ -1702,10 +1690,22 @@
     <t>D:\PrePayroll\2020\11\External\BOD</t>
   </si>
   <si>
-    <t>C10:AC;B9:D;0;B2:J;0;C2:F;B5:O;A4:F;D2:L;B2:K;B2:H</t>
-  </si>
-  <si>
-    <t>0,23,24,25,26;0,2,91,92,93;91,92,93,94,95;0,6,7,8,93;91,92,93,94,95;0,3,91,92,93;0,11,12,13,99;0,5,93,94,95;0,8,91,92,93;0,1,91,92,93;0,1,91,92,93</t>
+    <t>0;1000000;300000</t>
+  </si>
+  <si>
+    <t>4004,4005,4006,4007;4026;4003,4100;4001;0;2135;1000,1005,1010;2285;2060;2160;2190</t>
+  </si>
+  <si>
+    <t>C10:AC;B9:D;A2:D;B2:J;A2:C;C2:F;B5:O;A4:F;D2:L;B2:K;B2:H</t>
+  </si>
+  <si>
+    <t>0,23,24,25,26;0,2,91,92,93;0,2,3,94,95;0,6,7,8,93;0,2,93,94,95;0,3,91,92,93;0,11,12,13,99;0,5,93,94,95;0,8,91,92,93;0,1,91,92,93;0,1,91,92,93</t>
+  </si>
+  <si>
+    <t>8;8;1;1;1;1;4;3;1;1;1</t>
+  </si>
+  <si>
+    <t>ISAT 25 AGUSTUS 2020;Kopensat;ZIS;Overmedic;Fastel;Sheet1;New Hire;Meals;Musibah;Nikah;Khitan</t>
   </si>
 </sst>
 </file>
@@ -2172,8 +2172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1002"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2243,7 +2243,7 @@
         <v>13</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="I4" t="s">
         <v>515</v>
@@ -2305,7 +2305,7 @@
       <c r="A9" s="3">
         <v>2</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="21" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -2324,7 +2324,7 @@
         <v>22</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2360,7 +2360,7 @@
         <v>26</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2423,7 +2423,7 @@
       <c r="A16" s="3">
         <v>4</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="21" t="s">
         <v>33</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -2442,7 +2442,7 @@
         <v>36</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2478,7 +2478,7 @@
         <v>40</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -2502,7 +2502,7 @@
         <v>42</v>
       </c>
       <c r="D20" s="28" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>11</v>
@@ -2514,7 +2514,7 @@
         <v>44</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2559,7 +2559,7 @@
         <v>11</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2595,7 +2595,7 @@
         <v>50</v>
       </c>
       <c r="H26" s="26" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2612,7 +2612,7 @@
         <v>514</v>
       </c>
       <c r="H27" s="26" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2629,7 +2629,7 @@
         <v>512</v>
       </c>
       <c r="H28" s="26" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2637,16 +2637,16 @@
         <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C29" t="s">
         <v>513</v>
       </c>
       <c r="D29" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H29" s="26" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2654,16 +2654,16 @@
         <v>12</v>
       </c>
       <c r="B30" s="25" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="C30" s="30" t="s">
         <v>513</v>
       </c>
       <c r="D30" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="H30" s="26" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3649,7 +3649,7 @@
   <dimension ref="A4:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3663,7 +3663,7 @@
         <v>516</v>
       </c>
       <c r="B4" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -3671,7 +3671,7 @@
         <v>517</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -3695,23 +3695,23 @@
         <v>521</v>
       </c>
       <c r="B8" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>166</v>
       </c>
-      <c r="B9" t="s">
-        <v>552</v>
+      <c r="B9" s="31" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>522</v>
       </c>
-      <c r="B10" t="s">
-        <v>550</v>
+      <c r="B10" s="31" t="s">
+        <v>557</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -3719,7 +3719,7 @@
         <v>523</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -3727,23 +3727,23 @@
         <v>524</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>525</v>
       </c>
-      <c r="B13" t="s">
-        <v>551</v>
+      <c r="B13" s="31" t="s">
+        <v>556</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B14" t="s">
-        <v>526</v>
+        <v>552</v>
       </c>
     </row>
   </sheetData>
@@ -5313,7 +5313,7 @@
         <v>23</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D9" s="3">
         <v>4003</v>
@@ -5442,7 +5442,7 @@
         <v>41</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D18" s="3">
         <v>2135</v>
@@ -5725,7 +5725,7 @@
         <v>9</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>127</v>
@@ -5853,7 +5853,7 @@
         <v>143</v>
       </c>
       <c r="C47" s="21" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D47" s="5">
         <v>2155</v>
@@ -5968,7 +5968,7 @@
         <v>14</v>
       </c>
       <c r="B55" s="21" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>155</v>
@@ -6070,7 +6070,7 @@
         <v>163</v>
       </c>
       <c r="C62" s="21" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D62" s="3">
         <v>2330</v>

</xml_diff>